<commit_message>
thêm cột trạng thái đại lý cho toàn bộ báo cáo về đại lý
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Sales_Order_By_Store_And_Item.xlsx
+++ b/DMS/Templates/Report_Sales_Order_By_Store_And_Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6678042-CA56-49AC-AA60-E593308C3FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9620129-8B80-4A0F-A8BD-DC31A135EEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>STT</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>{{ReportSalesOrderByStoreAndItems.Stores.Items.SalesOrderCounter}}</t>
+  </si>
+  <si>
+    <t>Trạng thái đại lý</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByStoreAndItems.Stores.StoreStatusName}}</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,21 +632,23 @@
     <col min="4" max="4" width="6.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="20" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="7.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="28.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="14" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="15" style="3" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -653,8 +661,10 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -665,8 +675,10 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
-    <row r="4" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -686,28 +698,30 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
     </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
@@ -721,38 +735,42 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="17"/>
+      <c r="K7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
@@ -774,9 +792,11 @@
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
@@ -790,38 +810,42 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="19"/>
+      <c r="K9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="N9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="Q9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="R9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -835,36 +859,40 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="6"/>
+      <c r="Q10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="R10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="6"/>
+      <c r="S10" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="A8:T8"/>
+  <mergeCells count="15">
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A8:V8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
thêm mã tự nhập store các menu
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Sales_Order_By_Store_And_Item.xlsx
+++ b/DMS/Templates/Report_Sales_Order_By_Store_And_Item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9620129-8B80-4A0F-A8BD-DC31A135EEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85A78F6-B043-4BA7-81DC-7765E4B67BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>STT</t>
   </si>
@@ -126,9 +126,6 @@
     <t>{{ReportSalesOrderByStoreAndItems.Stores.Address}}</t>
   </si>
   <si>
-    <t>Mã đại lý</t>
-  </si>
-  <si>
     <t>Tên đại lý</t>
   </si>
   <si>
@@ -145,6 +142,15 @@
   </si>
   <si>
     <t>{{ReportSalesOrderByStoreAndItems.Stores.StoreStatusName}}</t>
+  </si>
+  <si>
+    <t>Mã đại lý (tự sinh)</t>
+  </si>
+  <si>
+    <t>Mã đại lý (tự nhập)</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderByStoreAndItems.Stores.CodeDraft}}</t>
   </si>
 </sst>
 </file>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,25 +636,27 @@
     <col min="1" max="2" width="5.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="28.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="14" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="15" style="3" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="13.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="15" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -663,8 +671,10 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -677,10 +687,12 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
-    <row r="4" spans="1:22" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -700,77 +712,85 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
     </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="16" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J7" s="17"/>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
@@ -794,9 +814,11 @@
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
-      <c r="V8" s="15"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="15"/>
     </row>
-    <row r="9" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
@@ -806,46 +828,50 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="18" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="18" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="19"/>
+      <c r="M9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="O9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="Q9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="R9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="T9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="8" t="s">
-        <v>37</v>
+      <c r="U9" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -861,38 +887,42 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="9" t="s">
+      <c r="R10" s="6"/>
+      <c r="S10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="T10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="S10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A8:V8"/>
+  <mergeCells count="17">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="A8:X8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I9:J9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>